<commit_message>
EPBDS-8351 added complex test for multirow
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/DataTables_Multirows.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/DataTables_Multirows.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F15809-C486-4539-98B3-1F10F785E72E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BD44B7-B520-44D7-B555-17152418F352}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="181">
   <si>
     <t>Datatype A</t>
   </si>
@@ -476,13 +476,103 @@
   </si>
   <si>
     <t>//Test proxyPolicy policyEL5</t>
+  </si>
+  <si>
+    <t>RiskItem[]</t>
+  </si>
+  <si>
+    <t>riskItems</t>
+  </si>
+  <si>
+    <t>Datatype RiskItem</t>
+  </si>
+  <si>
+    <t>Coverage[]</t>
+  </si>
+  <si>
+    <t>coverages</t>
+  </si>
+  <si>
+    <t>Datatype Coverage</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>Data Policy testPolicyCompexMr</t>
+  </si>
+  <si>
+    <t>riskItems.coverages.code</t>
+  </si>
+  <si>
+    <t>riskItems.name</t>
+  </si>
+  <si>
+    <t>riskItems.value</t>
+  </si>
+  <si>
+    <t>Coverage Code</t>
+  </si>
+  <si>
+    <t>Risk Item Name</t>
+  </si>
+  <si>
+    <t>Risk Item Value</t>
+  </si>
+  <si>
+    <t>Cov1</t>
+  </si>
+  <si>
+    <t>Risk1</t>
+  </si>
+  <si>
+    <t>Cov2</t>
+  </si>
+  <si>
+    <t>Risk2</t>
+  </si>
+  <si>
+    <t>Data Policy testPolicyCompexSr</t>
+  </si>
+  <si>
+    <t>riskItems[0].name</t>
+  </si>
+  <si>
+    <t>riskItems[0].value</t>
+  </si>
+  <si>
+    <t>riskItems[1].name</t>
+  </si>
+  <si>
+    <t>riskItems[1].value</t>
+  </si>
+  <si>
+    <t>riskItems[0].coverages[0].code</t>
+  </si>
+  <si>
+    <t>riskItems[0].coverages[1].code</t>
+  </si>
+  <si>
+    <t>riskItems[1].coverages[0].code</t>
+  </si>
+  <si>
+    <t>Method Policy proxyP(Policy p)</t>
+  </si>
+  <si>
+    <t>Test proxyP</t>
+  </si>
+  <si>
+    <t>&gt; testPolicyCompexMr</t>
+  </si>
+  <si>
+    <t>&gt; testPolicyCompexSr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -524,8 +614,20 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -571,6 +673,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -662,12 +770,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -730,6 +843,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -748,23 +870,49 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{81C4471A-A7AB-442F-A429-657424859F97}"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{59624ABA-F334-43A6-93B5-CB1AA879296D}"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{B8908434-AEC8-458C-BA1C-7E95CCF22A5B}"/>
+    <cellStyle name="Обычный 3" xfId="3" xr:uid="{E0C7485E-B2FE-4ED9-ABE5-E529D199A01B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1042,10 +1190,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:D28"/>
+  <dimension ref="C3:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,64 +1269,118 @@
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="27"/>
+      <c r="D20" s="39"/>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="38" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="38" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="38" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C26" s="27" t="s">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D24" s="38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="D26" s="27"/>
-    </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="16" t="s">
+      <c r="D27" s="39"/>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="38" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D28" s="38" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="16" t="s">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D29" s="38" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" s="39"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="38" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="D36" s="38" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C40" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="D40" s="39"/>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C41" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" s="38" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C40:D40"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C26:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1186,27 +1388,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4BD8076-7DC3-4701-B19A-D902A9B67FCD}">
-  <dimension ref="C3:H104"/>
+  <dimension ref="C3:I116"/>
   <sheetViews>
     <sheetView topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+      <selection activeCell="E124" sqref="E124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
       <c r="F3" s="26"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -1262,7 +1465,7 @@
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="28" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -1280,7 +1483,7 @@
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="35"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="7" t="s">
         <v>28</v>
       </c>
@@ -1294,7 +1497,7 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="28" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1312,7 +1515,7 @@
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="35"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="5" t="s">
         <v>19</v>
       </c>
@@ -1326,10 +1529,10 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="34" t="s">
+      <c r="D11" s="28" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -1344,8 +1547,8 @@
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
       <c r="E12" s="7" t="s">
         <v>37</v>
       </c>
@@ -1359,8 +1562,8 @@
       <c r="C16" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
       <c r="F16" s="26"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -1408,7 +1611,7 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="28" t="s">
         <v>23</v>
       </c>
       <c r="D20" s="8" t="s">
@@ -1420,7 +1623,7 @@
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="35"/>
+      <c r="C21" s="29"/>
       <c r="D21" s="7" t="s">
         <v>28</v>
       </c>
@@ -1430,7 +1633,7 @@
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="28" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -1442,7 +1645,7 @@
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="35"/>
+      <c r="C23" s="29"/>
       <c r="D23" s="5" t="s">
         <v>19</v>
       </c>
@@ -1452,10 +1655,10 @@
       </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="28" t="s">
         <v>21</v>
       </c>
       <c r="E24" s="8"/>
@@ -1464,8 +1667,8 @@
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7" t="s">
         <v>33</v>
@@ -1476,7 +1679,7 @@
       <c r="D29" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="36"/>
+      <c r="E29" s="30"/>
       <c r="F29" s="26"/>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.25">
@@ -1539,7 +1742,7 @@
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D35" s="34" t="s">
+      <c r="D35" s="28" t="s">
         <v>29</v>
       </c>
       <c r="E35" s="5" t="s">
@@ -1550,7 +1753,7 @@
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D36" s="35"/>
+      <c r="D36" s="29"/>
       <c r="E36" s="5" t="s">
         <v>26</v>
       </c>
@@ -1584,7 +1787,7 @@
       <c r="D42" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="36"/>
+      <c r="E42" s="30"/>
       <c r="F42" s="26"/>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.25">
@@ -1637,7 +1840,7 @@
       </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D48" s="34" t="s">
+      <c r="D48" s="28" t="s">
         <v>29</v>
       </c>
       <c r="E48" s="5"/>
@@ -1646,7 +1849,7 @@
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D49" s="35"/>
+      <c r="D49" s="29"/>
       <c r="E49" s="5"/>
       <c r="F49" s="4" t="s">
         <v>33</v>
@@ -1671,12 +1874,12 @@
       </c>
     </row>
     <row r="56" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D56" s="29" t="s">
+      <c r="D56" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="E56" s="30"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="31"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="34"/>
     </row>
     <row r="57" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D57" s="17" t="s">
@@ -1753,12 +1956,12 @@
       <c r="G62" s="24"/>
     </row>
     <row r="66" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D66" s="29" t="s">
+      <c r="D66" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="E66" s="30"/>
-      <c r="F66" s="30"/>
-      <c r="G66" s="31"/>
+      <c r="E66" s="33"/>
+      <c r="F66" s="33"/>
+      <c r="G66" s="34"/>
     </row>
     <row r="67" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D67" s="17" t="s">
@@ -1839,12 +2042,12 @@
       <c r="G72" s="24"/>
     </row>
     <row r="76" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D76" s="29" t="s">
+      <c r="D76" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="E76" s="30"/>
-      <c r="F76" s="30"/>
-      <c r="G76" s="31"/>
+      <c r="E76" s="33"/>
+      <c r="F76" s="33"/>
+      <c r="G76" s="34"/>
     </row>
     <row r="77" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D77" s="17" t="s">
@@ -1875,7 +2078,7 @@
       </c>
     </row>
     <row r="79" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D79" s="32" t="s">
+      <c r="D79" s="35" t="s">
         <v>118</v>
       </c>
       <c r="E79" s="21" t="s">
@@ -1887,7 +2090,7 @@
       <c r="G79" s="21"/>
     </row>
     <row r="80" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D80" s="32"/>
+      <c r="D80" s="35"/>
       <c r="E80" s="21" t="s">
         <v>119</v>
       </c>
@@ -1897,7 +2100,7 @@
       <c r="G80" s="21"/>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D81" s="28" t="s">
+      <c r="D81" s="31" t="s">
         <v>120</v>
       </c>
       <c r="E81" s="24" t="s">
@@ -1911,7 +2114,7 @@
       </c>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D82" s="28"/>
+      <c r="D82" s="31"/>
       <c r="E82" s="24" t="s">
         <v>122</v>
       </c>
@@ -1921,13 +2124,13 @@
       <c r="G82" s="24"/>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C86" s="29" t="s">
+      <c r="C86" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="D86" s="30"/>
-      <c r="E86" s="30"/>
-      <c r="F86" s="30"/>
-      <c r="G86" s="31"/>
+      <c r="D86" s="33"/>
+      <c r="E86" s="33"/>
+      <c r="F86" s="33"/>
+      <c r="G86" s="34"/>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C87" s="17" t="s">
@@ -1962,7 +2165,7 @@
       </c>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C89" s="33" t="s">
+      <c r="C89" s="36" t="s">
         <v>118</v>
       </c>
       <c r="D89" s="22" t="s">
@@ -1977,7 +2180,7 @@
       <c r="G89" s="21"/>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C90" s="33"/>
+      <c r="C90" s="36"/>
       <c r="D90" s="22" t="s">
         <v>127</v>
       </c>
@@ -1990,7 +2193,7 @@
       <c r="G90" s="21"/>
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="28" t="s">
+      <c r="C91" s="31" t="s">
         <v>120</v>
       </c>
       <c r="D91" s="23" t="s">
@@ -2007,7 +2210,7 @@
       </c>
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C92" s="28"/>
+      <c r="C92" s="31"/>
       <c r="D92" s="23" t="s">
         <v>129</v>
       </c>
@@ -2019,16 +2222,16 @@
       </c>
       <c r="G92" s="24"/>
     </row>
-    <row r="98" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C98" s="29" t="s">
+    <row r="98" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C98" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="D98" s="30"/>
-      <c r="E98" s="30"/>
-      <c r="F98" s="30"/>
-      <c r="G98" s="31"/>
-    </row>
-    <row r="99" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D98" s="33"/>
+      <c r="E98" s="33"/>
+      <c r="F98" s="33"/>
+      <c r="G98" s="34"/>
+    </row>
+    <row r="99" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C99" s="17" t="s">
         <v>125</v>
       </c>
@@ -2045,7 +2248,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="100" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C100" s="18"/>
       <c r="D100" s="18" t="s">
         <v>114</v>
@@ -2060,11 +2263,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="101" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C101" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="D101" s="33" t="s">
+      <c r="D101" s="36" t="s">
         <v>118</v>
       </c>
       <c r="E101" s="21" t="s">
@@ -2075,11 +2278,11 @@
       </c>
       <c r="G101" s="21"/>
     </row>
-    <row r="102" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C102" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D102" s="33"/>
+      <c r="D102" s="36"/>
       <c r="E102" s="21" t="s">
         <v>119</v>
       </c>
@@ -2088,11 +2291,11 @@
       </c>
       <c r="G102" s="21"/>
     </row>
-    <row r="103" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C103" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="D103" s="28" t="s">
+      <c r="D103" s="31" t="s">
         <v>120</v>
       </c>
       <c r="E103" s="24" t="s">
@@ -2105,11 +2308,11 @@
         <v>121</v>
       </c>
     </row>
-    <row r="104" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C104" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="D104" s="28"/>
+      <c r="D104" s="31"/>
       <c r="E104" s="24" t="s">
         <v>122</v>
       </c>
@@ -2118,8 +2321,168 @@
       </c>
       <c r="G104" s="24"/>
     </row>
+    <row r="109" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C109" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="D109" s="39"/>
+      <c r="E109" s="39"/>
+      <c r="F109" s="39"/>
+      <c r="G109" s="39"/>
+      <c r="H109" s="39"/>
+      <c r="I109" s="39"/>
+    </row>
+    <row r="110" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C110" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D110" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="E110" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="F110" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="G110" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="H110" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="I110" s="40" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="111" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C111" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="D111" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="E111" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="F111" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="G111" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="H111" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="I111" s="41" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="112" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C112" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="D112" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="E112" s="44">
+        <v>10</v>
+      </c>
+      <c r="F112" s="44"/>
+      <c r="G112" s="45" t="s">
+        <v>165</v>
+      </c>
+      <c r="H112" s="44" t="s">
+        <v>166</v>
+      </c>
+      <c r="I112" s="45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="113" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C113" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="D113" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="E113" s="44">
+        <v>20</v>
+      </c>
+      <c r="F113" s="44"/>
+      <c r="G113" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="H113" s="44" t="s">
+        <v>166</v>
+      </c>
+      <c r="I113" s="45">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="114" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C114" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="D114" s="44"/>
+      <c r="E114" s="44"/>
+      <c r="F114" s="44"/>
+      <c r="G114" s="45" t="s">
+        <v>165</v>
+      </c>
+      <c r="H114" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="I114" s="45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="115" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C115" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="D115" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="E115" s="43">
+        <v>30</v>
+      </c>
+      <c r="F115" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="G115" s="46"/>
+      <c r="H115" s="47"/>
+      <c r="I115" s="47"/>
+    </row>
+    <row r="116" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C116" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="D116" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="E116" s="43">
+        <v>40</v>
+      </c>
+      <c r="F116" s="43"/>
+      <c r="G116" s="46"/>
+      <c r="H116" s="47"/>
+      <c r="I116" s="47"/>
+    </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="26">
+    <mergeCell ref="C109:I109"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D66:G66"/>
+    <mergeCell ref="D76:G76"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="D101:D102"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C91:C92"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C3:F3"/>
@@ -2134,17 +2497,6 @@
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="C16:F16"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D66:G66"/>
-    <mergeCell ref="D76:G76"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="D101:D102"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="C91:C92"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2152,23 +2504,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC180073-2B4F-4898-B71D-AA553367764B}">
-  <dimension ref="C3:K55"/>
+  <dimension ref="C3:O64"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
@@ -2695,7 +3049,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C51" s="27" t="s">
         <v>144</v>
       </c>
@@ -2706,7 +3060,7 @@
       <c r="H51" s="27"/>
       <c r="I51" s="20"/>
     </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C52" s="16" t="s">
         <v>2</v>
       </c>
@@ -2726,7 +3080,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C53" s="16" t="s">
         <v>2</v>
       </c>
@@ -2746,7 +3100,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C54" s="16" t="s">
         <v>118</v>
       </c>
@@ -2764,7 +3118,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C55" s="16" t="s">
         <v>120</v>
       </c>
@@ -2784,8 +3138,174 @@
         <v>40</v>
       </c>
     </row>
+    <row r="60" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C60" s="39" t="s">
+        <v>169</v>
+      </c>
+      <c r="D60" s="39"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="39"/>
+      <c r="I60" s="39"/>
+      <c r="J60" s="39"/>
+      <c r="K60" s="39"/>
+      <c r="L60" s="39"/>
+      <c r="M60" s="39"/>
+      <c r="N60" s="39"/>
+      <c r="O60" s="39"/>
+    </row>
+    <row r="61" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C61" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="E61" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="F61" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="G61" s="48" t="s">
+        <v>133</v>
+      </c>
+      <c r="H61" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="I61" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="J61" s="48" t="s">
+        <v>171</v>
+      </c>
+      <c r="K61" s="48" t="s">
+        <v>172</v>
+      </c>
+      <c r="L61" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="M61" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="N61" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="O61" s="48" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="62" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C62" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="E62" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="F62" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="G62" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="H62" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="I62" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="J62" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="K62" s="49" t="s">
+        <v>163</v>
+      </c>
+      <c r="L62" s="49" t="s">
+        <v>164</v>
+      </c>
+      <c r="M62" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="N62" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="O62" s="49" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="63" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C63" s="51" t="s">
+        <v>118</v>
+      </c>
+      <c r="D63" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="E63" s="51">
+        <v>10</v>
+      </c>
+      <c r="F63" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="G63" s="51">
+        <v>20</v>
+      </c>
+      <c r="H63" s="51"/>
+      <c r="I63" s="51" t="s">
+        <v>166</v>
+      </c>
+      <c r="J63" s="51">
+        <v>100</v>
+      </c>
+      <c r="K63" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="L63" s="51">
+        <v>200</v>
+      </c>
+      <c r="M63" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="N63" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="O63" s="51" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="64" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C64" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="D64" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="E64" s="51">
+        <v>30</v>
+      </c>
+      <c r="F64" s="51" t="s">
+        <v>122</v>
+      </c>
+      <c r="G64" s="51">
+        <v>40</v>
+      </c>
+      <c r="H64" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="I64" s="51"/>
+      <c r="J64" s="51"/>
+      <c r="K64" s="51"/>
+      <c r="L64" s="51"/>
+      <c r="M64" s="51"/>
+      <c r="N64" s="51"/>
+      <c r="O64" s="51"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="C60:O60"/>
     <mergeCell ref="C3:K3"/>
     <mergeCell ref="C14:K14"/>
     <mergeCell ref="C25:G25"/>
@@ -2798,10 +3318,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C954F265-C4C4-48CF-B99C-CFD7F44F97B9}">
-  <dimension ref="C3:H88"/>
+  <dimension ref="C3:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3211,10 +3731,10 @@
       <c r="D44" s="27"/>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="29" t="s">
+      <c r="C47" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="D47" s="31"/>
+      <c r="D47" s="34"/>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="16" t="s">
@@ -3257,10 +3777,10 @@
       </c>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="29" t="s">
+      <c r="C56" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="D56" s="31"/>
+      <c r="D56" s="34"/>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C57" s="16" t="s">
@@ -3303,10 +3823,10 @@
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="29" t="s">
+      <c r="C65" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="D65" s="31"/>
+      <c r="D65" s="34"/>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C66" s="16" t="s">
@@ -3349,10 +3869,10 @@
       </c>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="29" t="s">
+      <c r="C74" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="D74" s="31"/>
+      <c r="D74" s="34"/>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C75" s="16" t="s">
@@ -3395,10 +3915,10 @@
       </c>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="29" t="s">
+      <c r="C83" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="D83" s="31"/>
+      <c r="D83" s="34"/>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C84" s="16" t="s">
@@ -3440,8 +3960,76 @@
         <v>120</v>
       </c>
     </row>
+    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C93" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="D93" s="39"/>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C94" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="D94" s="39"/>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C97" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="D97" s="39"/>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C98" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="D98" s="52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C99" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="D99" s="52" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C100" s="52" t="s">
+        <v>138</v>
+      </c>
+      <c r="D100" s="52" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C101" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="D101" s="52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C102" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="D102" s="52" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="17">
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C65:D65"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="C3:F3"/>
@@ -3449,13 +4037,6 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="F20:G20"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C65:D65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-8351 fix bug with PK for array element in multirows mode for Data tables
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/DataTables_Multirows.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/DataTables_Multirows.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BD44B7-B520-44D7-B555-17152418F352}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2B02C5-090E-4EDC-B087-12AEA576AE4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,18 +466,6 @@
     <t>&gt; testPolicyEL5</t>
   </si>
   <si>
-    <t>//Data Policy testPolicyEL5</t>
-  </si>
-  <si>
-    <t>//Data Policy testPolicyEL4</t>
-  </si>
-  <si>
-    <t>//Test proxyPolicy policyEL4</t>
-  </si>
-  <si>
-    <t>//Test proxyPolicy policyEL5</t>
-  </si>
-  <si>
     <t>RiskItem[]</t>
   </si>
   <si>
@@ -566,6 +554,18 @@
   </si>
   <si>
     <t>&gt; testPolicyCompexSr</t>
+  </si>
+  <si>
+    <t>Data Policy testPolicyEL5</t>
+  </si>
+  <si>
+    <t>Data Policy testPolicyEL4</t>
+  </si>
+  <si>
+    <t>Test proxyPolicy policyEL5</t>
+  </si>
+  <si>
+    <t>Test proxyPolicy policyEL4</t>
   </si>
 </sst>
 </file>
@@ -834,49 +834,7 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -906,6 +864,48 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{81C4471A-A7AB-442F-A429-657424859F97}"/>
@@ -1203,10 +1203,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="26"/>
+      <c r="D3" s="41"/>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
@@ -1225,10 +1225,10 @@
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="26"/>
+      <c r="D8" s="41"/>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
@@ -1247,10 +1247,10 @@
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="26"/>
+      <c r="D13" s="41"/>
     </row>
     <row r="14" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
@@ -1275,35 +1275,35 @@
       <c r="D20" s="39"/>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D22" s="25" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="38" t="s">
+      <c r="C23" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="25" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="D24" s="38" t="s">
-        <v>152</v>
+      <c r="C24" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
@@ -1313,74 +1313,74 @@
       <c r="D27" s="39"/>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C28" s="38" t="s">
+      <c r="C28" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="D28" s="38" t="s">
+      <c r="D28" s="25" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C29" s="38" t="s">
+      <c r="C29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" s="39" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D33" s="39"/>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D34" s="38" t="s">
+      <c r="D34" s="25" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="38" t="s">
+      <c r="C35" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="D35" s="38" t="s">
+      <c r="D35" s="25" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="38" t="s">
-        <v>154</v>
-      </c>
-      <c r="D36" s="38" t="s">
-        <v>155</v>
+      <c r="C36" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C40" s="39" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D40" s="39"/>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C41" s="38" t="s">
+      <c r="C41" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="38" t="s">
-        <v>157</v>
+      <c r="D41" s="25" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C3:D3"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1391,7 +1391,7 @@
   <dimension ref="C3:I116"/>
   <sheetViews>
     <sheetView topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="E124" sqref="E124"/>
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,12 +1405,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="26"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="41"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
@@ -1465,7 +1465,7 @@
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="48" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -1483,7 +1483,7 @@
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="29"/>
+      <c r="C8" s="49"/>
       <c r="D8" s="7" t="s">
         <v>28</v>
       </c>
@@ -1497,7 +1497,7 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="48" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1515,7 +1515,7 @@
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="29"/>
+      <c r="C10" s="49"/>
       <c r="D10" s="5" t="s">
         <v>19</v>
       </c>
@@ -1529,10 +1529,10 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="48" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -1547,8 +1547,8 @@
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="7" t="s">
         <v>37</v>
       </c>
@@ -1559,12 +1559,12 @@
       <c r="H12" s="2"/>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="26"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="41"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
@@ -1611,7 +1611,7 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="48" t="s">
         <v>23</v>
       </c>
       <c r="D20" s="8" t="s">
@@ -1623,7 +1623,7 @@
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="29"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="7" t="s">
         <v>28</v>
       </c>
@@ -1633,7 +1633,7 @@
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="48" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -1645,7 +1645,7 @@
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="29"/>
+      <c r="C23" s="49"/>
       <c r="D23" s="5" t="s">
         <v>19</v>
       </c>
@@ -1655,10 +1655,10 @@
       </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="48" t="s">
         <v>21</v>
       </c>
       <c r="E24" s="8"/>
@@ -1667,8 +1667,8 @@
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7" t="s">
         <v>33</v>
@@ -1676,11 +1676,11 @@
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="26"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="41"/>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C30" s="2"/>
@@ -1742,7 +1742,7 @@
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D35" s="28" t="s">
+      <c r="D35" s="48" t="s">
         <v>29</v>
       </c>
       <c r="E35" s="5" t="s">
@@ -1753,7 +1753,7 @@
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D36" s="29"/>
+      <c r="D36" s="49"/>
       <c r="E36" s="5" t="s">
         <v>26</v>
       </c>
@@ -1784,11 +1784,11 @@
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D42" s="25" t="s">
+      <c r="D42" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="30"/>
-      <c r="F42" s="26"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="41"/>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D43" s="3" t="s">
@@ -1840,7 +1840,7 @@
       </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D48" s="28" t="s">
+      <c r="D48" s="48" t="s">
         <v>29</v>
       </c>
       <c r="E48" s="5"/>
@@ -1849,7 +1849,7 @@
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D49" s="29"/>
+      <c r="D49" s="49"/>
       <c r="E49" s="5"/>
       <c r="F49" s="4" t="s">
         <v>33</v>
@@ -1874,12 +1874,12 @@
       </c>
     </row>
     <row r="56" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D56" s="32" t="s">
+      <c r="D56" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="E56" s="33"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="34"/>
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="45"/>
     </row>
     <row r="57" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D57" s="17" t="s">
@@ -1956,12 +1956,12 @@
       <c r="G62" s="24"/>
     </row>
     <row r="66" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D66" s="32" t="s">
+      <c r="D66" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="E66" s="33"/>
-      <c r="F66" s="33"/>
-      <c r="G66" s="34"/>
+      <c r="E66" s="44"/>
+      <c r="F66" s="44"/>
+      <c r="G66" s="45"/>
     </row>
     <row r="67" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D67" s="17" t="s">
@@ -2042,12 +2042,12 @@
       <c r="G72" s="24"/>
     </row>
     <row r="76" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D76" s="32" t="s">
+      <c r="D76" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="E76" s="33"/>
-      <c r="F76" s="33"/>
-      <c r="G76" s="34"/>
+      <c r="E76" s="44"/>
+      <c r="F76" s="44"/>
+      <c r="G76" s="45"/>
     </row>
     <row r="77" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D77" s="17" t="s">
@@ -2078,7 +2078,7 @@
       </c>
     </row>
     <row r="79" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D79" s="35" t="s">
+      <c r="D79" s="46" t="s">
         <v>118</v>
       </c>
       <c r="E79" s="21" t="s">
@@ -2090,7 +2090,7 @@
       <c r="G79" s="21"/>
     </row>
     <row r="80" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D80" s="35"/>
+      <c r="D80" s="46"/>
       <c r="E80" s="21" t="s">
         <v>119</v>
       </c>
@@ -2100,7 +2100,7 @@
       <c r="G80" s="21"/>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D81" s="31" t="s">
+      <c r="D81" s="42" t="s">
         <v>120</v>
       </c>
       <c r="E81" s="24" t="s">
@@ -2114,7 +2114,7 @@
       </c>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D82" s="31"/>
+      <c r="D82" s="42"/>
       <c r="E82" s="24" t="s">
         <v>122</v>
       </c>
@@ -2124,13 +2124,13 @@
       <c r="G82" s="24"/>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C86" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="D86" s="33"/>
-      <c r="E86" s="33"/>
-      <c r="F86" s="33"/>
-      <c r="G86" s="34"/>
+      <c r="C86" s="43" t="s">
+        <v>178</v>
+      </c>
+      <c r="D86" s="44"/>
+      <c r="E86" s="44"/>
+      <c r="F86" s="44"/>
+      <c r="G86" s="45"/>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C87" s="17" t="s">
@@ -2165,7 +2165,7 @@
       </c>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C89" s="36" t="s">
+      <c r="C89" s="47" t="s">
         <v>118</v>
       </c>
       <c r="D89" s="22" t="s">
@@ -2180,7 +2180,7 @@
       <c r="G89" s="21"/>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C90" s="36"/>
+      <c r="C90" s="47"/>
       <c r="D90" s="22" t="s">
         <v>127</v>
       </c>
@@ -2193,7 +2193,7 @@
       <c r="G90" s="21"/>
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="31" t="s">
+      <c r="C91" s="42" t="s">
         <v>120</v>
       </c>
       <c r="D91" s="23" t="s">
@@ -2210,7 +2210,7 @@
       </c>
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C92" s="31"/>
+      <c r="C92" s="42"/>
       <c r="D92" s="23" t="s">
         <v>129</v>
       </c>
@@ -2223,13 +2223,13 @@
       <c r="G92" s="24"/>
     </row>
     <row r="98" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C98" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="D98" s="33"/>
-      <c r="E98" s="33"/>
-      <c r="F98" s="33"/>
-      <c r="G98" s="34"/>
+      <c r="C98" s="43" t="s">
+        <v>177</v>
+      </c>
+      <c r="D98" s="44"/>
+      <c r="E98" s="44"/>
+      <c r="F98" s="44"/>
+      <c r="G98" s="45"/>
     </row>
     <row r="99" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C99" s="17" t="s">
@@ -2267,7 +2267,7 @@
       <c r="C101" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="D101" s="36" t="s">
+      <c r="D101" s="47" t="s">
         <v>118</v>
       </c>
       <c r="E101" s="21" t="s">
@@ -2282,7 +2282,7 @@
       <c r="C102" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D102" s="36"/>
+      <c r="D102" s="47"/>
       <c r="E102" s="21" t="s">
         <v>119</v>
       </c>
@@ -2295,7 +2295,7 @@
       <c r="C103" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="D103" s="31" t="s">
+      <c r="D103" s="42" t="s">
         <v>120</v>
       </c>
       <c r="E103" s="24" t="s">
@@ -2312,7 +2312,7 @@
       <c r="C104" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="D104" s="31"/>
+      <c r="D104" s="42"/>
       <c r="E104" s="24" t="s">
         <v>122</v>
       </c>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="109" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C109" s="39" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D109" s="39"/>
       <c r="E109" s="39"/>
@@ -2333,156 +2333,144 @@
       <c r="I109" s="39"/>
     </row>
     <row r="110" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C110" s="40" t="s">
+      <c r="C110" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D110" s="40" t="s">
+      <c r="D110" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="E110" s="40" t="s">
+      <c r="E110" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="F110" s="40" t="s">
+      <c r="F110" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="G110" s="40" t="s">
+      <c r="G110" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="H110" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="I110" s="26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="111" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C111" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D111" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E111" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="F111" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="G111" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="H111" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="H110" s="40" t="s">
+      <c r="I111" s="27" t="s">
         <v>160</v>
       </c>
-      <c r="I110" s="40" t="s">
+    </row>
+    <row r="112" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C112" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D112" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E112" s="30">
+        <v>10</v>
+      </c>
+      <c r="F112" s="30"/>
+      <c r="G112" s="31" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="111" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C111" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="D111" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="E111" s="42" t="s">
-        <v>116</v>
-      </c>
-      <c r="F111" s="41" t="s">
-        <v>117</v>
-      </c>
-      <c r="G111" s="41" t="s">
+      <c r="H112" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="H111" s="41" t="s">
+      <c r="I112" s="31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="113" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C113" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D113" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E113" s="30">
+        <v>20</v>
+      </c>
+      <c r="F113" s="30"/>
+      <c r="G113" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="I111" s="41" t="s">
+      <c r="H113" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="I113" s="31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="114" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C114" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="D114" s="30"/>
+      <c r="E114" s="30"/>
+      <c r="F114" s="30"/>
+      <c r="G114" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="H114" s="30" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="112" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C112" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="D112" s="44" t="s">
+      <c r="I114" s="31">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="115" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C115" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="D115" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="E112" s="44">
-        <v>10</v>
-      </c>
-      <c r="F112" s="44"/>
-      <c r="G112" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="H112" s="44" t="s">
-        <v>166</v>
-      </c>
-      <c r="I112" s="45">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="113" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C113" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="D113" s="44" t="s">
-        <v>119</v>
-      </c>
-      <c r="E113" s="44">
-        <v>20</v>
-      </c>
-      <c r="F113" s="44"/>
-      <c r="G113" s="45" t="s">
-        <v>167</v>
-      </c>
-      <c r="H113" s="44" t="s">
-        <v>166</v>
-      </c>
-      <c r="I113" s="45">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="114" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C114" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="D114" s="44"/>
-      <c r="E114" s="44"/>
-      <c r="F114" s="44"/>
-      <c r="G114" s="45" t="s">
-        <v>165</v>
-      </c>
-      <c r="H114" s="44" t="s">
-        <v>168</v>
-      </c>
-      <c r="I114" s="45">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="115" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C115" s="43" t="s">
+      <c r="E115" s="29">
+        <v>30</v>
+      </c>
+      <c r="F115" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="G115" s="32"/>
+      <c r="H115" s="33"/>
+      <c r="I115" s="33"/>
+    </row>
+    <row r="116" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C116" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="D115" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="E115" s="43">
-        <v>30</v>
-      </c>
-      <c r="F115" s="43" t="s">
-        <v>121</v>
-      </c>
-      <c r="G115" s="46"/>
-      <c r="H115" s="47"/>
-      <c r="I115" s="47"/>
-    </row>
-    <row r="116" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C116" s="43" t="s">
-        <v>120</v>
-      </c>
-      <c r="D116" s="43" t="s">
+      <c r="D116" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="E116" s="43">
+      <c r="E116" s="29">
         <v>40</v>
       </c>
-      <c r="F116" s="43"/>
-      <c r="G116" s="46"/>
-      <c r="H116" s="47"/>
-      <c r="I116" s="47"/>
+      <c r="F116" s="29"/>
+      <c r="G116" s="32"/>
+      <c r="H116" s="33"/>
+      <c r="I116" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C109:I109"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D66:G66"/>
-    <mergeCell ref="D76:G76"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="D101:D102"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="C91:C92"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C3:F3"/>
@@ -2497,6 +2485,18 @@
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C109:I109"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D66:G66"/>
+    <mergeCell ref="D76:G76"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="D101:D102"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C91:C92"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2506,8 +2506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC180073-2B4F-4898-B71D-AA553367764B}">
   <dimension ref="C3:O64"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I54" sqref="I54"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2526,17 +2526,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="10" t="s">
@@ -2681,17 +2681,17 @@
       <c r="K9" s="11"/>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C15" s="10" t="s">
@@ -2822,13 +2822,13 @@
       <c r="K20" s="11"/>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
@@ -2957,13 +2957,13 @@
       <c r="K31" s="9"/>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="37" t="s">
+      <c r="C36" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="10" t="s">
@@ -3050,14 +3050,14 @@
       </c>
     </row>
     <row r="51" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C51" s="27" t="s">
+      <c r="C51" s="52" t="s">
         <v>144</v>
       </c>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
+      <c r="D51" s="52"/>
+      <c r="E51" s="52"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="52"/>
+      <c r="H51" s="52"/>
       <c r="I51" s="20"/>
     </row>
     <row r="52" spans="3:15" x14ac:dyDescent="0.25">
@@ -3140,7 +3140,7 @@
     </row>
     <row r="60" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C60" s="39" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D60" s="39"/>
       <c r="E60" s="39"/>
@@ -3156,152 +3156,152 @@
       <c r="O60" s="39"/>
     </row>
     <row r="61" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C61" s="51" t="s">
+      <c r="C61" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="D61" s="48" t="s">
+      <c r="D61" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="E61" s="48" t="s">
+      <c r="E61" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="F61" s="48" t="s">
+      <c r="F61" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="G61" s="48" t="s">
+      <c r="G61" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="H61" s="48" t="s">
+      <c r="H61" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="I61" s="48" t="s">
+      <c r="I61" s="34" t="s">
+        <v>166</v>
+      </c>
+      <c r="J61" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="K61" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="L61" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="M61" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="J61" s="48" t="s">
+      <c r="N61" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="K61" s="48" t="s">
+      <c r="O61" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="L61" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="M61" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="N61" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="O61" s="48" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="62" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C62" s="49" t="s">
+      <c r="C62" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="D62" s="50" t="s">
+      <c r="D62" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="E62" s="50" t="s">
+      <c r="E62" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="F62" s="50" t="s">
+      <c r="F62" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="G62" s="50" t="s">
+      <c r="G62" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="H62" s="49" t="s">
+      <c r="H62" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="I62" s="49" t="s">
+      <c r="I62" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="J62" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="K62" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="L62" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="M62" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="N62" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="O62" s="35" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="63" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C63" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="D63" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="E63" s="37">
+        <v>10</v>
+      </c>
+      <c r="F63" s="37" t="s">
+        <v>119</v>
+      </c>
+      <c r="G63" s="37">
+        <v>20</v>
+      </c>
+      <c r="H63" s="37"/>
+      <c r="I63" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="J63" s="37">
+        <v>100</v>
+      </c>
+      <c r="K63" s="37" t="s">
+        <v>164</v>
+      </c>
+      <c r="L63" s="37">
+        <v>200</v>
+      </c>
+      <c r="M63" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="N63" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="J62" s="49" t="s">
-        <v>164</v>
-      </c>
-      <c r="K62" s="49" t="s">
-        <v>163</v>
-      </c>
-      <c r="L62" s="49" t="s">
-        <v>164</v>
-      </c>
-      <c r="M62" s="49" t="s">
-        <v>162</v>
-      </c>
-      <c r="N62" s="49" t="s">
-        <v>162</v>
-      </c>
-      <c r="O62" s="49" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="63" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C63" s="51" t="s">
-        <v>118</v>
-      </c>
-      <c r="D63" s="51" t="s">
+      <c r="O63" s="37" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="64" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C64" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="D64" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="E63" s="51">
-        <v>10</v>
-      </c>
-      <c r="F63" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="G63" s="51">
-        <v>20</v>
-      </c>
-      <c r="H63" s="51"/>
-      <c r="I63" s="51" t="s">
-        <v>166</v>
-      </c>
-      <c r="J63" s="51">
-        <v>100</v>
-      </c>
-      <c r="K63" s="51" t="s">
-        <v>168</v>
-      </c>
-      <c r="L63" s="51">
-        <v>200</v>
-      </c>
-      <c r="M63" s="51" t="s">
-        <v>165</v>
-      </c>
-      <c r="N63" s="51" t="s">
-        <v>167</v>
-      </c>
-      <c r="O63" s="51" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="64" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C64" s="51" t="s">
-        <v>120</v>
-      </c>
-      <c r="D64" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="E64" s="51">
+      <c r="E64" s="37">
         <v>30</v>
       </c>
-      <c r="F64" s="51" t="s">
+      <c r="F64" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="G64" s="51">
+      <c r="G64" s="37">
         <v>40</v>
       </c>
-      <c r="H64" s="51" t="s">
+      <c r="H64" s="37" t="s">
         <v>121</v>
       </c>
-      <c r="I64" s="51"/>
-      <c r="J64" s="51"/>
-      <c r="K64" s="51"/>
-      <c r="L64" s="51"/>
-      <c r="M64" s="51"/>
-      <c r="N64" s="51"/>
-      <c r="O64" s="51"/>
+      <c r="I64" s="37"/>
+      <c r="J64" s="37"/>
+      <c r="K64" s="37"/>
+      <c r="L64" s="37"/>
+      <c r="M64" s="37"/>
+      <c r="N64" s="37"/>
+      <c r="O64" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3321,7 +3321,7 @@
   <dimension ref="C3:H102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3334,12 +3334,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
       <c r="G3" s="13"/>
       <c r="H3" s="14" t="s">
         <v>62</v>
@@ -3444,15 +3444,15 @@
       <c r="H9" s="13"/>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="37"/>
+      <c r="D14" s="51"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="37" t="s">
+      <c r="F14" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="G14" s="37"/>
+      <c r="G14" s="51"/>
       <c r="H14" s="13"/>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
@@ -3487,15 +3487,15 @@
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="37"/>
+      <c r="D20" s="51"/>
       <c r="E20" s="13"/>
-      <c r="F20" s="37" t="s">
+      <c r="F20" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="G20" s="37"/>
+      <c r="G20" s="51"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="14" t="s">
@@ -3603,15 +3603,15 @@
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="D31" s="26"/>
+      <c r="D31" s="41"/>
       <c r="E31" s="13"/>
-      <c r="F31" s="25" t="s">
+      <c r="F31" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="G31" s="26"/>
+      <c r="G31" s="41"/>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="14" t="s">
@@ -3719,22 +3719,22 @@
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="27" t="s">
+      <c r="C43" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="27"/>
+      <c r="D43" s="52"/>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="27" t="s">
+      <c r="C44" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="D44" s="27"/>
+      <c r="D44" s="52"/>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="32" t="s">
+      <c r="C47" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="D47" s="34"/>
+      <c r="D47" s="45"/>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="16" t="s">
@@ -3777,10 +3777,10 @@
       </c>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="32" t="s">
+      <c r="C56" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="D56" s="34"/>
+      <c r="D56" s="45"/>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C57" s="16" t="s">
@@ -3823,10 +3823,10 @@
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="32" t="s">
+      <c r="C65" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="D65" s="34"/>
+      <c r="D65" s="45"/>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C66" s="16" t="s">
@@ -3869,10 +3869,10 @@
       </c>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="32" t="s">
-        <v>149</v>
-      </c>
-      <c r="D74" s="34"/>
+      <c r="C74" s="43" t="s">
+        <v>180</v>
+      </c>
+      <c r="D74" s="45"/>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C75" s="16" t="s">
@@ -3915,10 +3915,10 @@
       </c>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="32" t="s">
-        <v>150</v>
-      </c>
-      <c r="D83" s="34"/>
+      <c r="C83" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="D83" s="45"/>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C84" s="16" t="s">
@@ -3962,7 +3962,7 @@
     </row>
     <row r="93" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C93" s="39" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D93" s="39"/>
     </row>
@@ -3974,62 +3974,52 @@
     </row>
     <row r="97" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C97" s="39" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D97" s="39"/>
     </row>
     <row r="98" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C98" s="52" t="s">
+      <c r="C98" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="D98" s="52" t="s">
+      <c r="D98" s="38" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="99" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C99" s="52" t="s">
-        <v>179</v>
-      </c>
-      <c r="D99" s="52" t="s">
-        <v>180</v>
+      <c r="C99" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="D99" s="38" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="100" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C100" s="52" t="s">
+      <c r="C100" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="D100" s="52" t="s">
+      <c r="D100" s="38" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="101" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C101" s="52" t="s">
+      <c r="C101" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="D101" s="52" t="s">
+      <c r="D101" s="38" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="102" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C102" s="52" t="s">
+      <c r="C102" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="D102" s="52" t="s">
+      <c r="D102" s="38" t="s">
         <v>120</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C65:D65"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="C3:F3"/>
@@ -4037,6 +4027,16 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="F20:G20"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C83:D83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-8553 EPBDS-8555 EPBDS-8556 EPBDS-8558 update tests for Data tables
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/DataTables_Multirows.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/DataTables_Multirows.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2B02C5-090E-4EDC-B087-12AEA576AE4F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE944787-4BF6-4BF7-A820-E8641B0EB63E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datatypes" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="182">
   <si>
     <t>Datatype A</t>
   </si>
@@ -566,6 +566,9 @@
   </si>
   <si>
     <t>Test proxyPolicy policyEL4</t>
+  </si>
+  <si>
+    <t>cs._PK_</t>
   </si>
 </sst>
 </file>
@@ -617,6 +620,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -780,7 +784,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -864,13 +868,28 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -890,15 +909,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1203,10 +1213,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="41"/>
+      <c r="D3" s="42"/>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
@@ -1225,10 +1235,10 @@
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="41"/>
+      <c r="D8" s="42"/>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
@@ -1247,10 +1257,10 @@
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="41"/>
+      <c r="D13" s="42"/>
     </row>
     <row r="14" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
@@ -1269,10 +1279,10 @@
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="39"/>
+      <c r="D20" s="43"/>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C21" s="25" t="s">
@@ -1307,10 +1317,10 @@
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="39" t="s">
+      <c r="C27" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="39"/>
+      <c r="D27" s="43"/>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C28" s="25" t="s">
@@ -1329,10 +1339,10 @@
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="39" t="s">
+      <c r="C33" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="D33" s="39"/>
+      <c r="D33" s="43"/>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34" s="25" t="s">
@@ -1359,10 +1369,10 @@
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="39" t="s">
+      <c r="C40" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="D40" s="39"/>
+      <c r="D40" s="43"/>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C41" s="25" t="s">
@@ -1374,13 +1384,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1390,8 +1400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4BD8076-7DC3-4701-B19A-D902A9B67FCD}">
   <dimension ref="C3:I116"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,12 +1415,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="41"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="42"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
@@ -1465,7 +1475,7 @@
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="44" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -1483,7 +1493,7 @@
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="49"/>
+      <c r="C8" s="45"/>
       <c r="D8" s="7" t="s">
         <v>28</v>
       </c>
@@ -1497,7 +1507,7 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="44" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1515,7 +1525,7 @@
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="49"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="5" t="s">
         <v>19</v>
       </c>
@@ -1529,10 +1539,10 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="44" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -1547,8 +1557,8 @@
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
       <c r="E12" s="7" t="s">
         <v>37</v>
       </c>
@@ -1559,12 +1569,12 @@
       <c r="H12" s="2"/>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="41"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="42"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
@@ -1611,7 +1621,7 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="44" t="s">
         <v>23</v>
       </c>
       <c r="D20" s="8" t="s">
@@ -1623,7 +1633,7 @@
       </c>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="49"/>
+      <c r="C21" s="45"/>
       <c r="D21" s="7" t="s">
         <v>28</v>
       </c>
@@ -1633,7 +1643,7 @@
       </c>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="48" t="s">
+      <c r="C22" s="44" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -1645,7 +1655,7 @@
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="49"/>
+      <c r="C23" s="45"/>
       <c r="D23" s="5" t="s">
         <v>19</v>
       </c>
@@ -1655,10 +1665,10 @@
       </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="48" t="s">
+      <c r="D24" s="44" t="s">
         <v>21</v>
       </c>
       <c r="E24" s="8"/>
@@ -1667,8 +1677,8 @@
       </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7" t="s">
         <v>33</v>
@@ -1676,11 +1686,11 @@
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="50"/>
-      <c r="F29" s="41"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="42"/>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C30" s="2"/>
@@ -1718,7 +1728,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="2"/>
       <c r="D33" s="5" t="s">
         <v>23</v>
@@ -1730,7 +1740,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D34" s="5" t="s">
         <v>23</v>
       </c>
@@ -1741,8 +1751,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D35" s="48" t="s">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D35" s="44" t="s">
         <v>29</v>
       </c>
       <c r="E35" s="5" t="s">
@@ -1752,8 +1762,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D36" s="49"/>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D36" s="45"/>
       <c r="E36" s="5" t="s">
         <v>26</v>
       </c>
@@ -1761,7 +1771,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D37" s="5" t="s">
         <v>34</v>
       </c>
@@ -1772,7 +1782,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D38" s="5" t="s">
         <v>34</v>
       </c>
@@ -1783,75 +1793,97 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D42" s="40" t="s">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D42" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="50"/>
-      <c r="F42" s="41"/>
-    </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D43" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D44" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="G44" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D45" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7" t="s">
+      <c r="E45" s="7">
+        <v>1</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D46" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="5" t="s">
+      <c r="E46" s="5">
+        <v>2</v>
+      </c>
+      <c r="F46" s="4"/>
+      <c r="G46" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D47" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E47" s="4"/>
-      <c r="F47" s="5" t="s">
+      <c r="E47" s="5">
+        <v>3</v>
+      </c>
+      <c r="F47" s="4"/>
+      <c r="G47" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D48" s="48" t="s">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D48" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="4" t="s">
+      <c r="E48" s="39">
+        <v>4</v>
+      </c>
+      <c r="F48" s="5"/>
+      <c r="G48" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D49" s="49"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="4" t="s">
+      <c r="D49" s="45"/>
+      <c r="E49" s="40">
+        <v>5</v>
+      </c>
+      <c r="F49" s="5"/>
+      <c r="G49" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1859,8 +1891,11 @@
       <c r="D50" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E50" s="6"/>
-      <c r="F50" s="4" t="s">
+      <c r="E50" s="5">
+        <v>6</v>
+      </c>
+      <c r="F50" s="6"/>
+      <c r="G50" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1868,18 +1903,21 @@
       <c r="D51" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E51" s="6"/>
-      <c r="F51" s="4" t="s">
+      <c r="E51" s="5">
+        <v>7</v>
+      </c>
+      <c r="F51" s="6"/>
+      <c r="G51" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="56" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D56" s="43" t="s">
+      <c r="D56" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="E56" s="44"/>
-      <c r="F56" s="44"/>
-      <c r="G56" s="45"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="50"/>
     </row>
     <row r="57" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D57" s="17" t="s">
@@ -1956,12 +1994,12 @@
       <c r="G62" s="24"/>
     </row>
     <row r="66" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D66" s="43" t="s">
+      <c r="D66" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="E66" s="44"/>
-      <c r="F66" s="44"/>
-      <c r="G66" s="45"/>
+      <c r="E66" s="49"/>
+      <c r="F66" s="49"/>
+      <c r="G66" s="50"/>
     </row>
     <row r="67" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D67" s="17" t="s">
@@ -2042,12 +2080,12 @@
       <c r="G72" s="24"/>
     </row>
     <row r="76" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D76" s="43" t="s">
+      <c r="D76" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="E76" s="44"/>
-      <c r="F76" s="44"/>
-      <c r="G76" s="45"/>
+      <c r="E76" s="49"/>
+      <c r="F76" s="49"/>
+      <c r="G76" s="50"/>
     </row>
     <row r="77" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D77" s="17" t="s">
@@ -2078,7 +2116,7 @@
       </c>
     </row>
     <row r="79" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D79" s="46" t="s">
+      <c r="D79" s="51" t="s">
         <v>118</v>
       </c>
       <c r="E79" s="21" t="s">
@@ -2090,7 +2128,7 @@
       <c r="G79" s="21"/>
     </row>
     <row r="80" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D80" s="46"/>
+      <c r="D80" s="51"/>
       <c r="E80" s="21" t="s">
         <v>119</v>
       </c>
@@ -2100,7 +2138,7 @@
       <c r="G80" s="21"/>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D81" s="42" t="s">
+      <c r="D81" s="47" t="s">
         <v>120</v>
       </c>
       <c r="E81" s="24" t="s">
@@ -2114,7 +2152,7 @@
       </c>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D82" s="42"/>
+      <c r="D82" s="47"/>
       <c r="E82" s="24" t="s">
         <v>122</v>
       </c>
@@ -2124,13 +2162,13 @@
       <c r="G82" s="24"/>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C86" s="43" t="s">
+      <c r="C86" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="D86" s="44"/>
-      <c r="E86" s="44"/>
-      <c r="F86" s="44"/>
-      <c r="G86" s="45"/>
+      <c r="D86" s="49"/>
+      <c r="E86" s="49"/>
+      <c r="F86" s="49"/>
+      <c r="G86" s="50"/>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C87" s="17" t="s">
@@ -2165,7 +2203,7 @@
       </c>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C89" s="47" t="s">
+      <c r="C89" s="52" t="s">
         <v>118</v>
       </c>
       <c r="D89" s="22" t="s">
@@ -2180,7 +2218,7 @@
       <c r="G89" s="21"/>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C90" s="47"/>
+      <c r="C90" s="52"/>
       <c r="D90" s="22" t="s">
         <v>127</v>
       </c>
@@ -2193,7 +2231,7 @@
       <c r="G90" s="21"/>
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="42" t="s">
+      <c r="C91" s="47" t="s">
         <v>120</v>
       </c>
       <c r="D91" s="23" t="s">
@@ -2210,7 +2248,7 @@
       </c>
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C92" s="42"/>
+      <c r="C92" s="47"/>
       <c r="D92" s="23" t="s">
         <v>129</v>
       </c>
@@ -2223,13 +2261,13 @@
       <c r="G92" s="24"/>
     </row>
     <row r="98" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C98" s="43" t="s">
+      <c r="C98" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="D98" s="44"/>
-      <c r="E98" s="44"/>
-      <c r="F98" s="44"/>
-      <c r="G98" s="45"/>
+      <c r="D98" s="49"/>
+      <c r="E98" s="49"/>
+      <c r="F98" s="49"/>
+      <c r="G98" s="50"/>
     </row>
     <row r="99" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C99" s="17" t="s">
@@ -2267,7 +2305,7 @@
       <c r="C101" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="D101" s="47" t="s">
+      <c r="D101" s="52" t="s">
         <v>118</v>
       </c>
       <c r="E101" s="21" t="s">
@@ -2282,7 +2320,7 @@
       <c r="C102" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D102" s="47"/>
+      <c r="D102" s="52"/>
       <c r="E102" s="21" t="s">
         <v>119</v>
       </c>
@@ -2295,7 +2333,7 @@
       <c r="C103" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="D103" s="42" t="s">
+      <c r="D103" s="47" t="s">
         <v>120</v>
       </c>
       <c r="E103" s="24" t="s">
@@ -2312,7 +2350,7 @@
       <c r="C104" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="D104" s="42"/>
+      <c r="D104" s="47"/>
       <c r="E104" s="24" t="s">
         <v>122</v>
       </c>
@@ -2322,15 +2360,15 @@
       <c r="G104" s="24"/>
     </row>
     <row r="109" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C109" s="39" t="s">
+      <c r="C109" s="43" t="s">
         <v>154</v>
       </c>
-      <c r="D109" s="39"/>
-      <c r="E109" s="39"/>
-      <c r="F109" s="39"/>
-      <c r="G109" s="39"/>
-      <c r="H109" s="39"/>
-      <c r="I109" s="39"/>
+      <c r="D109" s="43"/>
+      <c r="E109" s="43"/>
+      <c r="F109" s="43"/>
+      <c r="G109" s="43"/>
+      <c r="H109" s="43"/>
+      <c r="I109" s="43"/>
     </row>
     <row r="110" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C110" s="26" t="s">
@@ -2471,20 +2509,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C16:F16"/>
     <mergeCell ref="C109:I109"/>
     <mergeCell ref="D103:D104"/>
     <mergeCell ref="D56:G56"/>
@@ -2497,6 +2521,20 @@
     <mergeCell ref="C86:G86"/>
     <mergeCell ref="C89:C90"/>
     <mergeCell ref="C91:C92"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="D42:G42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2526,17 +2564,17 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C4" s="10" t="s">
@@ -2681,17 +2719,17 @@
       <c r="K9" s="11"/>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="51" t="s">
+      <c r="C14" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C15" s="10" t="s">
@@ -2822,13 +2860,13 @@
       <c r="K20" s="11"/>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="51" t="s">
+      <c r="C25" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
@@ -2957,13 +2995,13 @@
       <c r="K31" s="9"/>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="51" t="s">
+      <c r="C36" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="10" t="s">
@@ -3050,14 +3088,14 @@
       </c>
     </row>
     <row r="51" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C51" s="52" t="s">
+      <c r="C51" s="54" t="s">
         <v>144</v>
       </c>
-      <c r="D51" s="52"/>
-      <c r="E51" s="52"/>
-      <c r="F51" s="52"/>
-      <c r="G51" s="52"/>
-      <c r="H51" s="52"/>
+      <c r="D51" s="54"/>
+      <c r="E51" s="54"/>
+      <c r="F51" s="54"/>
+      <c r="G51" s="54"/>
+      <c r="H51" s="54"/>
       <c r="I51" s="20"/>
     </row>
     <row r="52" spans="3:15" x14ac:dyDescent="0.25">
@@ -3139,21 +3177,21 @@
       </c>
     </row>
     <row r="60" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C60" s="39" t="s">
+      <c r="C60" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="D60" s="39"/>
-      <c r="E60" s="39"/>
-      <c r="F60" s="39"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="39"/>
-      <c r="I60" s="39"/>
-      <c r="J60" s="39"/>
-      <c r="K60" s="39"/>
-      <c r="L60" s="39"/>
-      <c r="M60" s="39"/>
-      <c r="N60" s="39"/>
-      <c r="O60" s="39"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="43"/>
+      <c r="H60" s="43"/>
+      <c r="I60" s="43"/>
+      <c r="J60" s="43"/>
+      <c r="K60" s="43"/>
+      <c r="L60" s="43"/>
+      <c r="M60" s="43"/>
+      <c r="N60" s="43"/>
+      <c r="O60" s="43"/>
     </row>
     <row r="61" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C61" s="37" t="s">
@@ -3320,7 +3358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C954F265-C4C4-48CF-B99C-CFD7F44F97B9}">
   <dimension ref="C3:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
@@ -3334,12 +3372,12 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
       <c r="G3" s="13"/>
       <c r="H3" s="14" t="s">
         <v>62</v>
@@ -3444,15 +3482,15 @@
       <c r="H9" s="13"/>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="51" t="s">
+      <c r="C14" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="51"/>
+      <c r="D14" s="53"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="51" t="s">
+      <c r="F14" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="G14" s="51"/>
+      <c r="G14" s="53"/>
       <c r="H14" s="13"/>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
@@ -3487,15 +3525,15 @@
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="51" t="s">
+      <c r="C20" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="51"/>
+      <c r="D20" s="53"/>
       <c r="E20" s="13"/>
-      <c r="F20" s="51" t="s">
+      <c r="F20" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="G20" s="51"/>
+      <c r="G20" s="53"/>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="14" t="s">
@@ -3603,15 +3641,15 @@
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="41" t="s">
         <v>98</v>
       </c>
-      <c r="D31" s="41"/>
+      <c r="D31" s="42"/>
       <c r="E31" s="13"/>
-      <c r="F31" s="40" t="s">
+      <c r="F31" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="G31" s="41"/>
+      <c r="G31" s="42"/>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="14" t="s">
@@ -3719,22 +3757,22 @@
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="52" t="s">
+      <c r="C43" s="54" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="52"/>
+      <c r="D43" s="54"/>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="52" t="s">
+      <c r="C44" s="54" t="s">
         <v>135</v>
       </c>
-      <c r="D44" s="52"/>
+      <c r="D44" s="54"/>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="43" t="s">
+      <c r="C47" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="D47" s="45"/>
+      <c r="D47" s="50"/>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="16" t="s">
@@ -3777,10 +3815,10 @@
       </c>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="43" t="s">
+      <c r="C56" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="D56" s="45"/>
+      <c r="D56" s="50"/>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C57" s="16" t="s">
@@ -3823,10 +3861,10 @@
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="43" t="s">
+      <c r="C65" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="D65" s="45"/>
+      <c r="D65" s="50"/>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C66" s="16" t="s">
@@ -3869,10 +3907,10 @@
       </c>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="43" t="s">
+      <c r="C74" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="D74" s="45"/>
+      <c r="D74" s="50"/>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C75" s="16" t="s">
@@ -3915,10 +3953,10 @@
       </c>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="43" t="s">
+      <c r="C83" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="D83" s="45"/>
+      <c r="D83" s="50"/>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C84" s="16" t="s">
@@ -3961,22 +3999,22 @@
       </c>
     </row>
     <row r="93" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C93" s="39" t="s">
+      <c r="C93" s="43" t="s">
         <v>173</v>
       </c>
-      <c r="D93" s="39"/>
+      <c r="D93" s="43"/>
     </row>
     <row r="94" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C94" s="39" t="s">
+      <c r="C94" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="D94" s="39"/>
+      <c r="D94" s="43"/>
     </row>
     <row r="97" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C97" s="39" t="s">
+      <c r="C97" s="43" t="s">
         <v>174</v>
       </c>
-      <c r="D97" s="39"/>
+      <c r="D97" s="43"/>
     </row>
     <row r="98" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C98" s="38" t="s">
@@ -4020,6 +4058,16 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C65:D65"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="C3:F3"/>
@@ -4027,16 +4075,6 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="F20:G20"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C83:D83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-8661 bug fix. no need to group rows in Data Tables if target class doesn't have a property with collection type
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/DataTables_Multirows.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/DataTables_Multirows.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE944787-4BF6-4BF7-A820-E8641B0EB63E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6714CA0-EF5A-4811-8683-09CD356FC044}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datatypes" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="181">
   <si>
     <t>Datatype A</t>
   </si>
@@ -566,9 +566,6 @@
   </si>
   <si>
     <t>Test proxyPolicy policyEL4</t>
-  </si>
-  <si>
-    <t>cs._PK_</t>
   </si>
 </sst>
 </file>
@@ -687,7 +684,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -773,6 +770,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -784,7 +790,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -868,28 +874,13 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -910,17 +901,27 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{81C4471A-A7AB-442F-A429-657424859F97}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{59624ABA-F334-43A6-93B5-CB1AA879296D}"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{B8908434-AEC8-458C-BA1C-7E95CCF22A5B}"/>
     <cellStyle name="Обычный 3" xfId="3" xr:uid="{E0C7485E-B2FE-4ED9-ABE5-E529D199A01B}"/>
   </cellStyles>
@@ -1206,19 +1207,19 @@
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="41" t="s">
+    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="42"/>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="41"/>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1226,7 +1227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1234,13 +1235,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="41" t="s">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C8" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="42"/>
-    </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="41"/>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1248,7 +1249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1256,13 +1257,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="41" t="s">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C13" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="42"/>
-    </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="41"/>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1270,7 +1271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
@@ -1278,13 +1279,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="43" t="s">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="43"/>
-    </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="39"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" s="25" t="s">
         <v>1</v>
       </c>
@@ -1292,7 +1293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" s="25" t="s">
         <v>1</v>
       </c>
@@ -1300,7 +1301,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C23" s="25" t="s">
         <v>106</v>
       </c>
@@ -1308,7 +1309,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24" s="25" t="s">
         <v>147</v>
       </c>
@@ -1316,13 +1317,13 @@
         <v>148</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C27" s="43" t="s">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C27" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="43"/>
-    </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="39"/>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C28" s="25" t="s">
         <v>109</v>
       </c>
@@ -1330,7 +1331,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C29" s="25" t="s">
         <v>1</v>
       </c>
@@ -1338,13 +1339,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="43" t="s">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C33" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="D33" s="43"/>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="39"/>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C34" s="25" t="s">
         <v>1</v>
       </c>
@@ -1352,7 +1353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C35" s="25" t="s">
         <v>109</v>
       </c>
@@ -1360,7 +1361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C36" s="25" t="s">
         <v>150</v>
       </c>
@@ -1368,13 +1369,13 @@
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C40" s="43" t="s">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C40" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="D40" s="43"/>
-    </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="39"/>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C41" s="25" t="s">
         <v>1</v>
       </c>
@@ -1400,31 +1401,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4BD8076-7DC3-4701-B19A-D902A9B67FCD}">
   <dimension ref="C3:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="41" t="s">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C3" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="42"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="41"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1440,7 +1441,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
@@ -1456,7 +1457,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C6" s="7" t="s">
         <v>18</v>
       </c>
@@ -1474,8 +1475,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="44" t="s">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C7" s="48" t="s">
         <v>23</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -1492,8 +1493,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="45"/>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C8" s="49"/>
       <c r="D8" s="7" t="s">
         <v>28</v>
       </c>
@@ -1506,8 +1507,8 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="44" t="s">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="48" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -1524,8 +1525,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="45"/>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C10" s="49"/>
       <c r="D10" s="5" t="s">
         <v>19</v>
       </c>
@@ -1538,11 +1539,11 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="44" t="s">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="48" t="s">
         <v>21</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -1556,9 +1557,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
       <c r="E12" s="7" t="s">
         <v>37</v>
       </c>
@@ -1568,17 +1569,17 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="41" t="s">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="42"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="41"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
         <v>2</v>
       </c>
@@ -1594,7 +1595,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
         <v>14</v>
       </c>
@@ -1608,7 +1609,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C19" s="7" t="s">
         <v>18</v>
       </c>
@@ -1620,8 +1621,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="44" t="s">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C20" s="48" t="s">
         <v>23</v>
       </c>
       <c r="D20" s="8" t="s">
@@ -1632,8 +1633,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="45"/>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C21" s="49"/>
       <c r="D21" s="7" t="s">
         <v>28</v>
       </c>
@@ -1642,8 +1643,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="44" t="s">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C22" s="48" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -1654,8 +1655,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="45"/>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C23" s="49"/>
       <c r="D23" s="5" t="s">
         <v>19</v>
       </c>
@@ -1664,11 +1665,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="44" t="s">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C24" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="48" t="s">
         <v>21</v>
       </c>
       <c r="E24" s="8"/>
@@ -1676,23 +1677,23 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C29" s="2"/>
-      <c r="D29" s="41" t="s">
+      <c r="D29" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="46"/>
-      <c r="F29" s="42"/>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="E29" s="50"/>
+      <c r="F29" s="41"/>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C30" s="2"/>
       <c r="D30" s="3" t="s">
         <v>2</v>
@@ -1704,7 +1705,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C31" s="2"/>
       <c r="D31" s="3" t="s">
         <v>15</v>
@@ -1716,7 +1717,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C32" s="2"/>
       <c r="D32" s="7" t="s">
         <v>18</v>
@@ -1728,7 +1729,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C33" s="2"/>
       <c r="D33" s="5" t="s">
         <v>23</v>
@@ -1740,7 +1741,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D34" s="5" t="s">
         <v>23</v>
       </c>
@@ -1751,8 +1752,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D35" s="44" t="s">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D35" s="48" t="s">
         <v>29</v>
       </c>
       <c r="E35" s="5" t="s">
@@ -1762,8 +1763,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D36" s="45"/>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D36" s="49"/>
       <c r="E36" s="5" t="s">
         <v>26</v>
       </c>
@@ -1771,7 +1772,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D37" s="5" t="s">
         <v>34</v>
       </c>
@@ -1782,7 +1783,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D38" s="5" t="s">
         <v>34</v>
       </c>
@@ -1793,133 +1794,106 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D42" s="53" t="s">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D42" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="53"/>
-      <c r="F42" s="53"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
       <c r="G42" s="53"/>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D43" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="14" t="s">
-        <v>181</v>
+      <c r="E43" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G43" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D44" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E44" s="14" t="s">
-        <v>181</v>
+      <c r="E44" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G44" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D45" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E45" s="7">
-        <v>1</v>
-      </c>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7" t="s">
+      <c r="E45" s="7"/>
+      <c r="F45" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D46" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E46" s="5">
-        <v>2</v>
-      </c>
-      <c r="F46" s="4"/>
-      <c r="G46" s="5" t="s">
+      <c r="E46" s="4"/>
+      <c r="F46" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.3">
       <c r="D47" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E47" s="5">
-        <v>3</v>
-      </c>
-      <c r="F47" s="4"/>
-      <c r="G47" s="5" t="s">
+      <c r="E47" s="4"/>
+      <c r="F47" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D48" s="44" t="s">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D48" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="E48" s="39">
-        <v>4</v>
-      </c>
-      <c r="F48" s="5"/>
-      <c r="G48" s="4" t="s">
+      <c r="E48" s="5"/>
+      <c r="F48" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D49" s="45"/>
-      <c r="E49" s="40">
-        <v>5</v>
-      </c>
-      <c r="F49" s="5"/>
-      <c r="G49" s="4" t="s">
+    <row r="49" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D49" s="49"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D50" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E50" s="5">
-        <v>6</v>
-      </c>
-      <c r="F50" s="6"/>
-      <c r="G50" s="4" t="s">
+      <c r="E50" s="6"/>
+      <c r="F50" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="51" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D51" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E51" s="5">
-        <v>7</v>
-      </c>
-      <c r="F51" s="6"/>
-      <c r="G51" s="4" t="s">
+      <c r="E51" s="6"/>
+      <c r="F51" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="56" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D56" s="48" t="s">
+    <row r="56" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D56" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="E56" s="49"/>
-      <c r="F56" s="49"/>
-      <c r="G56" s="50"/>
-    </row>
-    <row r="57" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E56" s="44"/>
+      <c r="F56" s="44"/>
+      <c r="G56" s="45"/>
+    </row>
+    <row r="57" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D57" s="17" t="s">
         <v>2</v>
       </c>
@@ -1933,7 +1907,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="58" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D58" s="18" t="s">
         <v>114</v>
       </c>
@@ -1947,7 +1921,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="59" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D59" s="21" t="s">
         <v>118</v>
       </c>
@@ -1959,7 +1933,7 @@
       </c>
       <c r="G59" s="21"/>
     </row>
-    <row r="60" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D60" s="21"/>
       <c r="E60" s="21" t="s">
         <v>119</v>
@@ -1969,7 +1943,7 @@
       </c>
       <c r="G60" s="21"/>
     </row>
-    <row r="61" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D61" s="24" t="s">
         <v>120</v>
       </c>
@@ -1983,7 +1957,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D62" s="24"/>
       <c r="E62" s="24" t="s">
         <v>122</v>
@@ -1993,15 +1967,15 @@
       </c>
       <c r="G62" s="24"/>
     </row>
-    <row r="66" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D66" s="48" t="s">
+    <row r="66" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D66" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="E66" s="49"/>
-      <c r="F66" s="49"/>
-      <c r="G66" s="50"/>
-    </row>
-    <row r="67" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E66" s="44"/>
+      <c r="F66" s="44"/>
+      <c r="G66" s="45"/>
+    </row>
+    <row r="67" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D67" s="17" t="s">
         <v>2</v>
       </c>
@@ -2015,7 +1989,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="68" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D68" s="18" t="s">
         <v>114</v>
       </c>
@@ -2029,7 +2003,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="69" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D69" s="21" t="s">
         <v>118</v>
       </c>
@@ -2041,7 +2015,7 @@
       </c>
       <c r="G69" s="21"/>
     </row>
-    <row r="70" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D70" s="21" t="s">
         <v>118</v>
       </c>
@@ -2053,7 +2027,7 @@
       </c>
       <c r="G70" s="21"/>
     </row>
-    <row r="71" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D71" s="24" t="s">
         <v>120</v>
       </c>
@@ -2067,7 +2041,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="72" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D72" s="24" t="s">
         <v>120</v>
       </c>
@@ -2079,15 +2053,15 @@
       </c>
       <c r="G72" s="24"/>
     </row>
-    <row r="76" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D76" s="48" t="s">
+    <row r="76" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D76" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="E76" s="49"/>
-      <c r="F76" s="49"/>
-      <c r="G76" s="50"/>
-    </row>
-    <row r="77" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E76" s="44"/>
+      <c r="F76" s="44"/>
+      <c r="G76" s="45"/>
+    </row>
+    <row r="77" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D77" s="17" t="s">
         <v>2</v>
       </c>
@@ -2101,7 +2075,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="78" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D78" s="18" t="s">
         <v>114</v>
       </c>
@@ -2115,8 +2089,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D79" s="51" t="s">
+    <row r="79" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D79" s="46" t="s">
         <v>118</v>
       </c>
       <c r="E79" s="21" t="s">
@@ -2127,8 +2101,8 @@
       </c>
       <c r="G79" s="21"/>
     </row>
-    <row r="80" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D80" s="51"/>
+    <row r="80" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D80" s="46"/>
       <c r="E80" s="21" t="s">
         <v>119</v>
       </c>
@@ -2137,8 +2111,8 @@
       </c>
       <c r="G80" s="21"/>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D81" s="47" t="s">
+    <row r="81" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D81" s="42" t="s">
         <v>120</v>
       </c>
       <c r="E81" s="24" t="s">
@@ -2151,8 +2125,8 @@
         <v>121</v>
       </c>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D82" s="47"/>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="D82" s="42"/>
       <c r="E82" s="24" t="s">
         <v>122</v>
       </c>
@@ -2161,16 +2135,16 @@
       </c>
       <c r="G82" s="24"/>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C86" s="48" t="s">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C86" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="D86" s="49"/>
-      <c r="E86" s="49"/>
-      <c r="F86" s="49"/>
-      <c r="G86" s="50"/>
-    </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D86" s="44"/>
+      <c r="E86" s="44"/>
+      <c r="F86" s="44"/>
+      <c r="G86" s="45"/>
+    </row>
+    <row r="87" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C87" s="17" t="s">
         <v>2</v>
       </c>
@@ -2187,7 +2161,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C88" s="18" t="s">
         <v>114</v>
       </c>
@@ -2202,8 +2176,8 @@
         <v>117</v>
       </c>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C89" s="52" t="s">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C89" s="47" t="s">
         <v>118</v>
       </c>
       <c r="D89" s="22" t="s">
@@ -2217,8 +2191,8 @@
       </c>
       <c r="G89" s="21"/>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C90" s="52"/>
+    <row r="90" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C90" s="47"/>
       <c r="D90" s="22" t="s">
         <v>127</v>
       </c>
@@ -2230,8 +2204,8 @@
       </c>
       <c r="G90" s="21"/>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="47" t="s">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C91" s="42" t="s">
         <v>120</v>
       </c>
       <c r="D91" s="23" t="s">
@@ -2247,8 +2221,8 @@
         <v>121</v>
       </c>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C92" s="47"/>
+    <row r="92" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C92" s="42"/>
       <c r="D92" s="23" t="s">
         <v>129</v>
       </c>
@@ -2260,16 +2234,16 @@
       </c>
       <c r="G92" s="24"/>
     </row>
-    <row r="98" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C98" s="48" t="s">
+    <row r="98" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C98" s="43" t="s">
         <v>177</v>
       </c>
-      <c r="D98" s="49"/>
-      <c r="E98" s="49"/>
-      <c r="F98" s="49"/>
-      <c r="G98" s="50"/>
-    </row>
-    <row r="99" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D98" s="44"/>
+      <c r="E98" s="44"/>
+      <c r="F98" s="44"/>
+      <c r="G98" s="45"/>
+    </row>
+    <row r="99" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C99" s="17" t="s">
         <v>125</v>
       </c>
@@ -2286,7 +2260,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="100" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C100" s="18"/>
       <c r="D100" s="18" t="s">
         <v>114</v>
@@ -2301,11 +2275,11 @@
         <v>117</v>
       </c>
     </row>
-    <row r="101" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C101" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="D101" s="52" t="s">
+      <c r="D101" s="47" t="s">
         <v>118</v>
       </c>
       <c r="E101" s="21" t="s">
@@ -2316,11 +2290,11 @@
       </c>
       <c r="G101" s="21"/>
     </row>
-    <row r="102" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C102" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="D102" s="52"/>
+      <c r="D102" s="47"/>
       <c r="E102" s="21" t="s">
         <v>119</v>
       </c>
@@ -2329,11 +2303,11 @@
       </c>
       <c r="G102" s="21"/>
     </row>
-    <row r="103" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C103" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="D103" s="47" t="s">
+      <c r="D103" s="42" t="s">
         <v>120</v>
       </c>
       <c r="E103" s="24" t="s">
@@ -2346,11 +2320,11 @@
         <v>121</v>
       </c>
     </row>
-    <row r="104" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C104" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="D104" s="47"/>
+      <c r="D104" s="42"/>
       <c r="E104" s="24" t="s">
         <v>122</v>
       </c>
@@ -2359,18 +2333,18 @@
       </c>
       <c r="G104" s="24"/>
     </row>
-    <row r="109" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C109" s="43" t="s">
+    <row r="109" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C109" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="D109" s="43"/>
-      <c r="E109" s="43"/>
-      <c r="F109" s="43"/>
-      <c r="G109" s="43"/>
-      <c r="H109" s="43"/>
-      <c r="I109" s="43"/>
-    </row>
-    <row r="110" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D109" s="39"/>
+      <c r="E109" s="39"/>
+      <c r="F109" s="39"/>
+      <c r="G109" s="39"/>
+      <c r="H109" s="39"/>
+      <c r="I109" s="39"/>
+    </row>
+    <row r="110" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C110" s="26" t="s">
         <v>2</v>
       </c>
@@ -2393,7 +2367,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="111" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C111" s="27" t="s">
         <v>114</v>
       </c>
@@ -2416,7 +2390,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="112" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C112" s="30" t="s">
         <v>118</v>
       </c>
@@ -2437,7 +2411,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="113" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C113" s="30" t="s">
         <v>118</v>
       </c>
@@ -2458,7 +2432,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="114" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C114" s="30" t="s">
         <v>118</v>
       </c>
@@ -2475,7 +2449,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="115" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C115" s="29" t="s">
         <v>120</v>
       </c>
@@ -2492,7 +2466,7 @@
       <c r="H115" s="33"/>
       <c r="I115" s="33"/>
     </row>
-    <row r="116" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C116" s="29" t="s">
         <v>120</v>
       </c>
@@ -2509,18 +2483,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C109:I109"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="D56:G56"/>
-    <mergeCell ref="D66:G66"/>
-    <mergeCell ref="D76:G76"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="C98:G98"/>
-    <mergeCell ref="D101:D102"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="C91:C92"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C3:F3"/>
@@ -2534,7 +2496,19 @@
     <mergeCell ref="D11:D12"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="C16:F16"/>
-    <mergeCell ref="D42:G42"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="C109:I109"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="D56:G56"/>
+    <mergeCell ref="D66:G66"/>
+    <mergeCell ref="D76:G76"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="C98:G98"/>
+    <mergeCell ref="D101:D102"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C91:C92"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2548,35 +2522,35 @@
       <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="26.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C3" s="53" t="s">
+    <row r="3" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C3" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-    </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C4" s="10" t="s">
         <v>2</v>
       </c>
@@ -2605,7 +2579,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C5" s="10" t="s">
         <v>14</v>
       </c>
@@ -2628,7 +2602,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C6" s="12" t="s">
         <v>18</v>
       </c>
@@ -2647,7 +2621,7 @@
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C7" s="12" t="s">
         <v>23</v>
       </c>
@@ -2672,7 +2646,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C8" s="12" t="s">
         <v>29</v>
       </c>
@@ -2695,7 +2669,7 @@
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
     </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C9" s="12" t="s">
         <v>34</v>
       </c>
@@ -2718,20 +2692,20 @@
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
     </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C14" s="53" t="s">
+    <row r="14" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C14" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-    </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C15" s="10" t="s">
         <v>2</v>
       </c>
@@ -2760,7 +2734,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C16" s="10" t="s">
         <v>14</v>
       </c>
@@ -2783,7 +2757,7 @@
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C17" s="12" t="s">
         <v>18</v>
       </c>
@@ -2800,7 +2774,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="11"/>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C18" s="12" t="s">
         <v>23</v>
       </c>
@@ -2821,7 +2795,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C19" s="12" t="s">
         <v>29</v>
       </c>
@@ -2840,7 +2814,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="11"/>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C20" s="12" t="s">
         <v>34</v>
       </c>
@@ -2859,20 +2833,20 @@
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
     </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C25" s="53" t="s">
+    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="C25" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="53"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="51"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
     </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C26" s="10" t="s">
         <v>2</v>
       </c>
@@ -2893,7 +2867,7 @@
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
     </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C27" s="10" t="s">
         <v>15</v>
       </c>
@@ -2914,7 +2888,7 @@
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
     </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C28" s="11" t="s">
         <v>18</v>
       </c>
@@ -2931,7 +2905,7 @@
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
     </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C29" s="11" t="s">
         <v>23</v>
       </c>
@@ -2952,7 +2926,7 @@
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
     </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C30" s="11" t="s">
         <v>29</v>
       </c>
@@ -2973,7 +2947,7 @@
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
     </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C31" s="12" t="s">
         <v>34</v>
       </c>
@@ -2994,16 +2968,16 @@
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="53" t="s">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C36" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="D36" s="53"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
-      <c r="G36" s="53"/>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C37" s="10" t="s">
         <v>2</v>
       </c>
@@ -3020,7 +2994,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C38" s="10" t="s">
         <v>15</v>
       </c>
@@ -3037,7 +3011,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C39" s="11" t="s">
         <v>18</v>
       </c>
@@ -3048,7 +3022,7 @@
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C40" s="11" t="s">
         <v>23</v>
       </c>
@@ -3061,7 +3035,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C41" s="11" t="s">
         <v>29</v>
       </c>
@@ -3074,7 +3048,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C42" s="12" t="s">
         <v>34</v>
       </c>
@@ -3087,18 +3061,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C51" s="54" t="s">
+    <row r="51" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C51" s="52" t="s">
         <v>144</v>
       </c>
-      <c r="D51" s="54"/>
-      <c r="E51" s="54"/>
-      <c r="F51" s="54"/>
-      <c r="G51" s="54"/>
-      <c r="H51" s="54"/>
+      <c r="D51" s="52"/>
+      <c r="E51" s="52"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="52"/>
+      <c r="H51" s="52"/>
       <c r="I51" s="20"/>
     </row>
-    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C52" s="16" t="s">
         <v>2</v>
       </c>
@@ -3118,7 +3092,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C53" s="16" t="s">
         <v>2</v>
       </c>
@@ -3138,7 +3112,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="54" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C54" s="16" t="s">
         <v>118</v>
       </c>
@@ -3156,7 +3130,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C55" s="16" t="s">
         <v>120</v>
       </c>
@@ -3176,24 +3150,24 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C60" s="43" t="s">
+    <row r="60" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C60" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="D60" s="43"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="43"/>
-      <c r="H60" s="43"/>
-      <c r="I60" s="43"/>
-      <c r="J60" s="43"/>
-      <c r="K60" s="43"/>
-      <c r="L60" s="43"/>
-      <c r="M60" s="43"/>
-      <c r="N60" s="43"/>
-      <c r="O60" s="43"/>
-    </row>
-    <row r="61" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="D60" s="39"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="39"/>
+      <c r="H60" s="39"/>
+      <c r="I60" s="39"/>
+      <c r="J60" s="39"/>
+      <c r="K60" s="39"/>
+      <c r="L60" s="39"/>
+      <c r="M60" s="39"/>
+      <c r="N60" s="39"/>
+      <c r="O60" s="39"/>
+    </row>
+    <row r="61" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C61" s="37" t="s">
         <v>2</v>
       </c>
@@ -3234,7 +3208,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="62" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C62" s="35" t="s">
         <v>114</v>
       </c>
@@ -3275,7 +3249,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="63" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C63" s="37" t="s">
         <v>118</v>
       </c>
@@ -3314,7 +3288,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="64" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C64" s="37" t="s">
         <v>120</v>
       </c>
@@ -3362,28 +3336,28 @@
       <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="53" t="s">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C3" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
       <c r="G3" s="13"/>
       <c r="H3" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C4" s="14" t="s">
         <v>63</v>
       </c>
@@ -3401,7 +3375,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C5" s="14" t="s">
         <v>68</v>
       </c>
@@ -3419,7 +3393,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C6" s="14" t="s">
         <v>73</v>
       </c>
@@ -3437,7 +3411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7" s="14" t="s">
         <v>76</v>
       </c>
@@ -3453,7 +3427,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8" s="14" t="s">
         <v>79</v>
       </c>
@@ -3469,7 +3443,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9" s="14" t="s">
         <v>82</v>
       </c>
@@ -3481,19 +3455,19 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="53" t="s">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="51" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="53"/>
+      <c r="D14" s="51"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="53" t="s">
+      <c r="F14" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="G14" s="53"/>
+      <c r="G14" s="51"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C15" s="14" t="s">
         <v>63</v>
       </c>
@@ -3509,7 +3483,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C16" s="14" t="s">
         <v>86</v>
       </c>
@@ -3524,18 +3498,18 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="53" t="s">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C20" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="53"/>
+      <c r="D20" s="51"/>
       <c r="E20" s="13"/>
-      <c r="F20" s="53" t="s">
+      <c r="F20" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="G20" s="53"/>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="51"/>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C21" s="14" t="s">
         <v>90</v>
       </c>
@@ -3550,7 +3524,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C22" s="14" t="s">
         <v>92</v>
       </c>
@@ -3565,7 +3539,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C23" s="14" t="s">
         <v>96</v>
       </c>
@@ -3580,7 +3554,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C24" s="14" t="s">
         <v>18</v>
       </c>
@@ -3595,7 +3569,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C25" s="14" t="s">
         <v>23</v>
       </c>
@@ -3610,7 +3584,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C26" s="14" t="s">
         <v>29</v>
       </c>
@@ -3625,7 +3599,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C27" s="14" t="s">
         <v>34</v>
       </c>
@@ -3640,18 +3614,18 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="41" t="s">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C31" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="D31" s="42"/>
+      <c r="D31" s="41"/>
       <c r="E31" s="13"/>
-      <c r="F31" s="41" t="s">
+      <c r="F31" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="G31" s="42"/>
-    </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="41"/>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C32" s="14" t="s">
         <v>90</v>
       </c>
@@ -3666,7 +3640,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C33" s="14" t="s">
         <v>100</v>
       </c>
@@ -3681,7 +3655,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C34" s="14" t="s">
         <v>96</v>
       </c>
@@ -3696,7 +3670,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C35" s="14" t="s">
         <v>18</v>
       </c>
@@ -3711,7 +3685,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C36" s="14" t="s">
         <v>23</v>
       </c>
@@ -3726,7 +3700,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C37" s="14" t="s">
         <v>29</v>
       </c>
@@ -3741,7 +3715,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C38" s="14" t="s">
         <v>34</v>
       </c>
@@ -3756,25 +3730,25 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="54" t="s">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C43" s="52" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="54"/>
-    </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="54" t="s">
+      <c r="D43" s="52"/>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C44" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="D44" s="54"/>
-    </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="48" t="s">
+      <c r="D44" s="52"/>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C47" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="D47" s="50"/>
-    </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D47" s="45"/>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C48" s="16" t="s">
         <v>138</v>
       </c>
@@ -3782,7 +3756,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49" s="16" t="s">
         <v>137</v>
       </c>
@@ -3790,7 +3764,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50" s="16" t="s">
         <v>138</v>
       </c>
@@ -3798,7 +3772,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C51" s="16" t="s">
         <v>118</v>
       </c>
@@ -3806,7 +3780,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C52" s="16" t="s">
         <v>120</v>
       </c>
@@ -3814,13 +3788,13 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C56" s="48" t="s">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C56" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="D56" s="50"/>
-    </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="45"/>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C57" s="16" t="s">
         <v>138</v>
       </c>
@@ -3828,7 +3802,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C58" s="16" t="s">
         <v>140</v>
       </c>
@@ -3836,7 +3810,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C59" s="16" t="s">
         <v>138</v>
       </c>
@@ -3844,7 +3818,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C60" s="16" t="s">
         <v>118</v>
       </c>
@@ -3852,7 +3826,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C61" s="16" t="s">
         <v>120</v>
       </c>
@@ -3860,13 +3834,13 @@
         <v>120</v>
       </c>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" s="48" t="s">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C65" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="D65" s="50"/>
-    </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="45"/>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C66" s="16" t="s">
         <v>138</v>
       </c>
@@ -3874,7 +3848,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C67" s="16" t="s">
         <v>143</v>
       </c>
@@ -3882,7 +3856,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C68" s="16" t="s">
         <v>138</v>
       </c>
@@ -3890,7 +3864,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C69" s="16" t="s">
         <v>118</v>
       </c>
@@ -3898,7 +3872,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C70" s="16" t="s">
         <v>120</v>
       </c>
@@ -3906,13 +3880,13 @@
         <v>120</v>
       </c>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C74" s="48" t="s">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C74" s="43" t="s">
         <v>180</v>
       </c>
-      <c r="D74" s="50"/>
-    </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D74" s="45"/>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C75" s="16" t="s">
         <v>138</v>
       </c>
@@ -3920,7 +3894,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C76" s="16" t="s">
         <v>145</v>
       </c>
@@ -3928,7 +3902,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C77" s="16" t="s">
         <v>138</v>
       </c>
@@ -3936,7 +3910,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C78" s="16" t="s">
         <v>118</v>
       </c>
@@ -3944,7 +3918,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C79" s="16" t="s">
         <v>120</v>
       </c>
@@ -3952,13 +3926,13 @@
         <v>120</v>
       </c>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C83" s="48" t="s">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C83" s="43" t="s">
         <v>179</v>
       </c>
-      <c r="D83" s="50"/>
-    </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="45"/>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C84" s="16" t="s">
         <v>138</v>
       </c>
@@ -3966,7 +3940,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C85" s="16" t="s">
         <v>146</v>
       </c>
@@ -3974,7 +3948,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C86" s="16" t="s">
         <v>138</v>
       </c>
@@ -3982,7 +3956,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C87" s="16" t="s">
         <v>118</v>
       </c>
@@ -3990,7 +3964,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C88" s="16" t="s">
         <v>120</v>
       </c>
@@ -3998,25 +3972,25 @@
         <v>120</v>
       </c>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C93" s="43" t="s">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C93" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="D93" s="43"/>
-    </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C94" s="43" t="s">
+      <c r="D93" s="39"/>
+    </row>
+    <row r="94" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C94" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="D94" s="43"/>
-    </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C97" s="43" t="s">
+      <c r="D94" s="39"/>
+    </row>
+    <row r="97" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C97" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="D97" s="43"/>
-    </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D97" s="39"/>
+    </row>
+    <row r="98" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C98" s="38" t="s">
         <v>138</v>
       </c>
@@ -4024,7 +3998,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C99" s="38" t="s">
         <v>175</v>
       </c>
@@ -4032,7 +4006,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C100" s="38" t="s">
         <v>138</v>
       </c>
@@ -4040,7 +4014,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C101" s="38" t="s">
         <v>118</v>
       </c>
@@ -4048,7 +4022,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C102" s="38" t="s">
         <v>120</v>
       </c>
@@ -4058,16 +4032,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C65:D65"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="C3:F3"/>
@@ -4075,6 +4039,16 @@
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="F20:G20"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C83:D83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>